<commit_message>
- updated excel file
</commit_message>
<xml_diff>
--- a/public/admin_assets/sample/ot_hostel_excel_upload.xlsx
+++ b/public/admin_assets/sample/ot_hostel_excel_upload.xlsx
@@ -20,12 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">course_master_pk</t>
+  </si>
   <si>
     <t xml:space="preserve">user_name</t>
   </si>
   <si>
     <t xml:space="preserve">hostel_room_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JayasreePradhan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SILV-102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mundrawhat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAHA-104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akankshapathak1509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeepeshKaira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SILV-302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prakharkr29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negiitushar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rana_ananya04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suramyasharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SILV-301</t>
   </si>
 </sst>
 </file>
@@ -107,13 +146,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -305,26 +352,119 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>